<commit_message>
workout and Intel SDM
</commit_message>
<xml_diff>
--- a/work/workout.xlsx
+++ b/work/workout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\code\work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ACEC024-7287-4E61-A158-0E3F6FE64FED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A176E5-C84C-4AA5-8214-A187906BC235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{723923E2-2CA0-49AA-84BB-AEB574CEA5B6}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>Exercise</t>
   </si>
@@ -47,18 +47,12 @@
     <t>Day 1</t>
   </si>
   <si>
-    <t>Incline bench press</t>
-  </si>
-  <si>
     <t>Seated DB shoulder press</t>
   </si>
   <si>
     <t>Day 2</t>
   </si>
   <si>
-    <t>Romanian deadlift</t>
-  </si>
-  <si>
     <t>Seated leg curls</t>
   </si>
   <si>
@@ -125,10 +119,13 @@
     <t>knee on bench - straight up</t>
   </si>
   <si>
-    <t>find machine</t>
-  </si>
-  <si>
-    <t>bar rolls on leg</t>
+    <t>Incline chest press</t>
+  </si>
+  <si>
+    <t>freebie</t>
+  </si>
+  <si>
+    <t>fix 3/30</t>
   </si>
 </sst>
 </file>
@@ -539,9 +536,7 @@
   </sheetPr>
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N19" sqref="N19"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -555,40 +550,40 @@
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5"/>
+      <c r="B2" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="C2" s="3" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="D2" s="7">
         <v>40</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>28</v>
-      </c>
+      <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3" s="7">
         <v>15</v>
@@ -598,29 +593,29 @@
     <row r="4" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D4" s="7">
         <v>40</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="5"/>
       <c r="C5" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D5" s="7">
         <v>5</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -632,60 +627,58 @@
     </row>
     <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="7">
-        <v>60</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>29</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D8" s="7">
         <v>30</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D9" s="7">
         <v>50</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D10" s="7">
         <v>30</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -697,60 +690,60 @@
     </row>
     <row r="12" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D12" s="7">
         <v>60</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="5"/>
       <c r="C13" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D13" s="7">
         <v>20</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D14" s="7">
         <v>35</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="5"/>
       <c r="C15" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D15" s="7">
         <v>10</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
debug notes and workout
</commit_message>
<xml_diff>
--- a/work/workout.xlsx
+++ b/work/workout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\code\work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A176E5-C84C-4AA5-8214-A187906BC235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1E82BEA-EFAA-4E5C-91AD-B375A84C4633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{723923E2-2CA0-49AA-84BB-AEB574CEA5B6}"/>
   </bookViews>
@@ -39,29 +39,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>Exercise</t>
   </si>
   <si>
-    <t>Day 1</t>
-  </si>
-  <si>
-    <t>Seated DB shoulder press</t>
-  </si>
-  <si>
-    <t>Day 2</t>
-  </si>
-  <si>
     <t>Seated leg curls</t>
   </si>
   <si>
     <t>Leg extensions</t>
   </si>
   <si>
-    <t>Day 3</t>
-  </si>
-  <si>
     <t>Neutral grip pulldowns</t>
   </si>
   <si>
@@ -89,12 +77,6 @@
     <t>machine</t>
   </si>
   <si>
-    <t>Pecs</t>
-  </si>
-  <si>
-    <t>pec machine</t>
-  </si>
-  <si>
     <t>pull up machine</t>
   </si>
   <si>
@@ -107,12 +89,6 @@
     <t>x</t>
   </si>
   <si>
-    <t>Seated DB lateral raises</t>
-  </si>
-  <si>
-    <t>wings lift up</t>
-  </si>
-  <si>
     <t>Leg press</t>
   </si>
   <si>
@@ -126,6 +102,24 @@
   </si>
   <si>
     <t>fix 3/30</t>
+  </si>
+  <si>
+    <t>Shoulder press</t>
+  </si>
+  <si>
+    <t>Tricep press</t>
+  </si>
+  <si>
+    <t>Lateral raises</t>
+  </si>
+  <si>
+    <t>Mon</t>
+  </si>
+  <si>
+    <t>Wed</t>
+  </si>
+  <si>
+    <t>Fri</t>
   </si>
 </sst>
 </file>
@@ -536,7 +530,9 @@
   </sheetPr>
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -550,27 +546,27 @@
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D2" s="7">
         <v>40</v>
@@ -580,10 +576,10 @@
     <row r="3" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>2</v>
       </c>
       <c r="D3" s="7">
         <v>15</v>
@@ -593,30 +589,28 @@
     <row r="4" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D4" s="7">
-        <v>40</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>17</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
-      <c r="B5" s="5"/>
+      <c r="B5" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="C5" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" s="7">
-        <v>5</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>23</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
@@ -627,11 +621,11 @@
     </row>
     <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="3" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="3"/>
@@ -639,46 +633,46 @@
     <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D8" s="7">
         <v>30</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D9" s="7">
         <v>50</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D10" s="7">
         <v>30</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -690,60 +684,60 @@
     </row>
     <row r="12" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D12" s="7">
         <v>60</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="5"/>
       <c r="C13" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D13" s="7">
         <v>20</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D14" s="7">
         <v>35</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="5"/>
       <c r="C15" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D15" s="7">
         <v>10</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
debug and workout updates
</commit_message>
<xml_diff>
--- a/work/workout.xlsx
+++ b/work/workout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\code\work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85428824-B7C5-4F2C-8DB7-9191C4ABDDDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD85CA8-9825-430F-ABE5-E4A6B418E7E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{723923E2-2CA0-49AA-84BB-AEB574CEA5B6}"/>
   </bookViews>
@@ -39,14 +39,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>Exercise</t>
   </si>
   <si>
-    <t>Seated leg curls</t>
-  </si>
-  <si>
     <t>Leg extensions</t>
   </si>
   <si>
@@ -62,9 +59,6 @@
     <t>x</t>
   </si>
   <si>
-    <t>Leg press</t>
-  </si>
-  <si>
     <t>Shoulder press</t>
   </si>
   <si>
@@ -95,10 +89,19 @@
     <t>1-arm DB rows (knee on bench straight up)</t>
   </si>
   <si>
-    <t>biceps</t>
-  </si>
-  <si>
     <t>Chest press</t>
+  </si>
+  <si>
+    <t>Ab Crunch</t>
+  </si>
+  <si>
+    <t>Linear leg press</t>
+  </si>
+  <si>
+    <t>3x45 each side</t>
+  </si>
+  <si>
+    <t>Kneeling leg curls</t>
   </si>
 </sst>
 </file>
@@ -143,7 +146,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -166,11 +169,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -190,6 +204,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -510,7 +530,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,195 +539,194 @@
     <col min="2" max="2" width="9.140625" style="6"/>
     <col min="3" max="3" width="49.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5703125" style="8" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" style="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D2" s="7">
         <v>40</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="11"/>
     </row>
     <row r="3" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>8</v>
       </c>
       <c r="D3" s="7">
         <v>30</v>
       </c>
-      <c r="E3" s="3"/>
+      <c r="E3" s="11"/>
     </row>
     <row r="4" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D4" s="7">
         <v>90</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="11"/>
     </row>
     <row r="5" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D5" s="7">
         <v>20</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="E5" s="11"/>
     </row>
     <row r="6" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="5"/>
       <c r="C6" s="3"/>
       <c r="D6" s="7"/>
-      <c r="E6" s="3"/>
+      <c r="E6" s="11"/>
     </row>
     <row r="7" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D7" s="7">
-        <v>65</v>
-      </c>
-      <c r="E7" s="3"/>
+        <v>50</v>
+      </c>
+      <c r="E7" s="11"/>
     </row>
     <row r="8" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D8" s="7">
         <v>30</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="11"/>
     </row>
     <row r="9" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D9" s="7">
-        <v>50</v>
-      </c>
-      <c r="E9" s="3"/>
+        <v>270</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="7">
-        <v>30</v>
-      </c>
-      <c r="E10" s="3"/>
+      <c r="C10" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="8">
+        <v>0</v>
+      </c>
+      <c r="E10" s="11"/>
     </row>
     <row r="11" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="5"/>
       <c r="C11" s="3"/>
       <c r="D11" s="7"/>
-      <c r="E11" s="3"/>
+      <c r="E11" s="11"/>
     </row>
     <row r="12" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D12" s="7">
         <v>80</v>
       </c>
-      <c r="E12" s="3"/>
+      <c r="E12" s="11"/>
     </row>
     <row r="13" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="5"/>
       <c r="C13" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D13" s="7">
         <v>30</v>
       </c>
-      <c r="E13" s="3"/>
+      <c r="E13" s="11"/>
     </row>
     <row r="14" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D14" s="7">
         <v>35</v>
       </c>
-      <c r="E14" s="3"/>
+      <c r="E14" s="11"/>
     </row>
     <row r="15" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="5"/>
       <c r="C15" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D15" s="7">
         <v>10</v>
       </c>
-      <c r="E15" s="3"/>
+      <c r="E15" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update to camera class lower filter
</commit_message>
<xml_diff>
--- a/work/workout.xlsx
+++ b/work/workout.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\code\work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C92B9DD9-E03F-42C4-9622-B2C4FAD9B5DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0232EB04-3D74-4F16-9F98-EC71139F6907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{723923E2-2CA0-49AA-84BB-AEB574CEA5B6}"/>
   </bookViews>
@@ -548,7 +548,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,7 +612,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="5">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="D4" s="5">
         <v>20</v>
@@ -673,7 +673,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="5">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="9"/>
@@ -738,7 +738,7 @@
         <v>22</v>
       </c>
       <c r="C15" s="5">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="9"/>

</xml_diff>